<commit_message>
added file exports for raw datasets
</commit_message>
<xml_diff>
--- a/Quality reports shared/seed distribution.xlsx
+++ b/Quality reports shared/seed distribution.xlsx
@@ -2248,7 +2248,7 @@
         <v>120</v>
       </c>
       <c r="I58">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2306,7 +2306,7 @@
         <v>120</v>
       </c>
       <c r="I60">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3866,7 +3866,7 @@
         <v>505</v>
       </c>
       <c r="I114">
-        <v>490</v>
+        <v>495</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -3895,7 +3895,7 @@
         <v>40</v>
       </c>
       <c r="I115">
-        <v>39.2</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -3950,7 +3950,7 @@
         <v>101</v>
       </c>
       <c r="I117">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4289,7 +4289,7 @@
         <v>117</v>
       </c>
       <c r="I129">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4854,7 +4854,7 @@
         <v>238</v>
       </c>
       <c r="I149">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -5080,7 +5080,7 @@
         <v>70</v>
       </c>
       <c r="I157">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="158" spans="1:9">

</xml_diff>